<commit_message>
fix: fixed excel file
</commit_message>
<xml_diff>
--- a/src/assets/template-report-department.xlsx
+++ b/src/assets/template-report-department.xlsx
@@ -127,11 +127,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Libre Franklin"/>
     </font>
     <font/>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Libre Franklin"/>
+    </font>
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -145,12 +151,6 @@
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Libre Franklin"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Libre Franklin"/>
@@ -175,7 +175,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border/>
     <border>
       <bottom style="thin">
@@ -248,110 +248,101 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="5" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="0" fontId="6" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="5" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="7" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -603,461 +594,497 @@
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="3"/>
-      <c r="J1" s="4" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
+      <c r="J1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="7"/>
     </row>
     <row r="2" ht="15.0" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="3"/>
-      <c r="J2" s="9" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="4"/>
+      <c r="J2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="7"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="3"/>
-      <c r="J3" s="10" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="4"/>
+      <c r="J3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="11" t="s">
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="6"/>
+      <c r="O3" s="7"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="3"/>
-      <c r="J4" s="10" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="4"/>
+      <c r="J4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="11">
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="13">
         <v>1.7</v>
       </c>
-      <c r="O4" s="6"/>
+      <c r="O4" s="7"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="3"/>
-      <c r="J5" s="10" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="4"/>
+      <c r="J5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="11">
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="13">
         <v>6.0</v>
       </c>
-      <c r="O5" s="6"/>
+      <c r="O5" s="7"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="3"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="4"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="3"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="6"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="4"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="3"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="4"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="3"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
+      <c r="A9" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
+      <c r="A10" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="16" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="16" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="16" t="s">
-        <v>14</v>
-      </c>
+      <c r="A13" s="20"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="16" t="s">
-        <v>15</v>
-      </c>
+      <c r="A14" s="20"/>
     </row>
     <row r="15" ht="24.0" customHeight="1">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="12"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="14"/>
     </row>
     <row r="16" ht="27.75" customHeight="1">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="18" t="s">
+      <c r="H16" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="18" t="s">
+      <c r="I16" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="J16" s="18" t="s">
+      <c r="J16" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="K16" s="19" t="s">
+      <c r="K16" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="L16" s="5"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="18" t="s">
+      <c r="L16" s="6"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="O16" s="18" t="s">
+      <c r="O16" s="22" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" ht="27.75" customHeight="1">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="18" t="s">
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="L17" s="18" t="s">
+      <c r="L17" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="M17" s="18" t="s">
+      <c r="M17" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="N17" s="20"/>
-      <c r="O17" s="20"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
     </row>
     <row r="18" ht="27.75" customHeight="1">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="21"/>
-      <c r="O18" s="21"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="25"/>
+      <c r="N18" s="25"/>
+      <c r="O18" s="25"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="22"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="24"/>
+      <c r="A20" s="26"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="22"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="24"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="22"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="24"/>
-      <c r="O22" s="24"/>
+      <c r="A22" s="26"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="28"/>
+      <c r="O22" s="28"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="32"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="28"/>
-      <c r="N23" s="24"/>
-      <c r="O23" s="24"/>
+      <c r="A23" s="36"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
+      <c r="N23" s="28"/>
+      <c r="O23" s="28"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="22"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="24"/>
-      <c r="O24" s="24"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="22"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="27"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="24"/>
-      <c r="O25" s="24"/>
-      <c r="P25" s="12"/>
-      <c r="Q25" s="12"/>
-      <c r="W25" s="12"/>
-      <c r="X25" s="12"/>
-      <c r="Y25" s="12"/>
-      <c r="Z25" s="12"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="28"/>
+      <c r="O25" s="28"/>
+      <c r="P25" s="14"/>
+      <c r="Q25" s="14"/>
+      <c r="W25" s="14"/>
+      <c r="X25" s="14"/>
+      <c r="Y25" s="14"/>
+      <c r="Z25" s="14"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="22"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="24"/>
-      <c r="O26" s="24"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="28"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="33"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="27"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="12"/>
-      <c r="Q27" s="12"/>
-      <c r="W27" s="12"/>
-      <c r="X27" s="12"/>
-      <c r="Y27" s="12"/>
-      <c r="Z27" s="12"/>
+      <c r="A27" s="37"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="28"/>
+      <c r="O27" s="28"/>
+      <c r="P27" s="14"/>
+      <c r="Q27" s="14"/>
+      <c r="W27" s="14"/>
+      <c r="X27" s="14"/>
+      <c r="Y27" s="14"/>
+      <c r="Z27" s="14"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="33"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="27"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="24"/>
-      <c r="O28" s="24"/>
-      <c r="P28" s="34"/>
-      <c r="Q28" s="34"/>
-      <c r="W28" s="34"/>
-      <c r="X28" s="34"/>
-      <c r="Y28" s="34"/>
-      <c r="Z28" s="34"/>
+      <c r="A28" s="37"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="28"/>
+      <c r="P28" s="32"/>
+      <c r="Q28" s="32"/>
+      <c r="W28" s="32"/>
+      <c r="X28" s="32"/>
+      <c r="Y28" s="32"/>
+      <c r="Z28" s="32"/>
     </row>
     <row r="29" ht="15.75" customHeight="1"/>
     <row r="30" ht="15.75" customHeight="1"/>
@@ -2032,45 +2059,47 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
+  <mergeCells count="40">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="J2:O2"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="A13:O13"/>
+    <mergeCell ref="A14:O14"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="N4:O4"/>
     <mergeCell ref="J5:M5"/>
     <mergeCell ref="N5:O5"/>
     <mergeCell ref="J6:M6"/>
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="J7:O7"/>
-    <mergeCell ref="A11:O11"/>
-    <mergeCell ref="A12:O12"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="N16:N18"/>
+    <mergeCell ref="O16:O18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="E16:E18"/>
     <mergeCell ref="F16:F18"/>
     <mergeCell ref="G16:G18"/>
     <mergeCell ref="H16:H18"/>
     <mergeCell ref="I16:I18"/>
     <mergeCell ref="J16:J18"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="N16:N18"/>
-    <mergeCell ref="O16:O18"/>
-    <mergeCell ref="A13:O13"/>
-    <mergeCell ref="A14:O14"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="E16:E18"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="J2:O2"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="N4:O4"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.7480314960629921" footer="0.0" header="0.0" left="0.3937007874015748" right="0.31496062992125984" top="1.6535433070866143"/>
@@ -2092,7 +2121,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="7.63"/>
+    <col customWidth="1" min="1" max="6" width="7.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1"/>
@@ -3113,7 +3142,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="7.63"/>
+    <col customWidth="1" min="1" max="6" width="7.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
fix: added new param in file
</commit_message>
<xml_diff>
--- a/src/assets/template-report-department.xlsx
+++ b/src/assets/template-report-department.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Наименование предприятия</t>
   </si>
@@ -36,19 +36,16 @@
     <t xml:space="preserve">Katana 210 QS </t>
   </si>
   <si>
-    <t>Ответственное лицо</t>
+    <t>ФИО</t>
   </si>
   <si>
     <t>Индекс рефракции</t>
   </si>
   <si>
-    <t>ФИО</t>
+    <t>Должность</t>
   </si>
   <si>
     <t>Рекомендуемая концентрация эмульсии, %</t>
-  </si>
-  <si>
-    <t>Должность</t>
   </si>
   <si>
     <t>Тип оборудования</t>
@@ -57,7 +54,7 @@
     <t>Модель</t>
   </si>
   <si>
-    <t>Инвентарный номер</t>
+    <t>Номер станка</t>
   </si>
   <si>
     <t xml:space="preserve"> Емкость системы СОЖ (л)</t>
@@ -74,9 +71,6 @@
   <si>
     <t>Электропроводность
 µS/cm</t>
-  </si>
-  <si>
-    <t>Уровень эмульсии в баке, л</t>
   </si>
   <si>
     <t>Долив (л)</t>
@@ -100,26 +94,17 @@
     <t>Примечания и рекомендации</t>
   </si>
   <si>
-    <t>Номер партии СОЖ</t>
-  </si>
-  <si>
     <t>Фунгицид</t>
   </si>
   <si>
     <t>Биоцид</t>
-  </si>
-  <si>
-    <t>Пеногаситель</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -139,11 +124,6 @@
       <name val="Libre Franklin"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Open Sans"/>
-    </font>
-    <font>
       <b/>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -153,11 +133,6 @@
       <u/>
       <sz val="11.0"/>
       <color theme="1"/>
-      <name val="Libre Franklin"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
       <name val="Libre Franklin"/>
     </font>
   </fonts>
@@ -175,7 +150,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border/>
     <border>
       <bottom style="thin">
@@ -202,6 +177,20 @@
       </bottom>
     </border>
     <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -252,20 +241,19 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="6" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -276,18 +264,25 @@
     <xf borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="5" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="bottom"/>
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="bottom"/>
@@ -301,48 +296,15 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -572,20 +534,19 @@
     <col customWidth="1" min="1" max="1" width="10.25"/>
     <col customWidth="1" min="2" max="2" width="8.88"/>
     <col customWidth="1" min="3" max="3" width="5.88"/>
-    <col customWidth="1" min="4" max="5" width="9.25"/>
-    <col customWidth="1" min="6" max="6" width="9.38"/>
-    <col customWidth="1" min="7" max="7" width="7.63"/>
-    <col customWidth="1" min="8" max="8" width="7.13"/>
-    <col customWidth="1" min="9" max="9" width="7.75"/>
-    <col customWidth="1" min="10" max="10" width="12.88"/>
-    <col customWidth="1" min="11" max="13" width="8.25"/>
-    <col customWidth="1" min="14" max="14" width="29.13"/>
-    <col customWidth="1" min="15" max="15" width="10.13"/>
-    <col customWidth="1" min="16" max="18" width="7.63"/>
-    <col customWidth="1" min="19" max="19" width="2.38"/>
-    <col customWidth="1" min="20" max="20" width="11.13"/>
-    <col customWidth="1" min="21" max="21" width="12.0"/>
-    <col customWidth="1" min="22" max="26" width="7.63"/>
+    <col customWidth="1" min="4" max="4" width="9.25"/>
+    <col customWidth="1" min="5" max="5" width="9.38"/>
+    <col customWidth="1" min="6" max="6" width="7.63"/>
+    <col customWidth="1" min="7" max="7" width="7.13"/>
+    <col customWidth="1" min="8" max="8" width="7.75"/>
+    <col customWidth="1" min="9" max="9" width="12.88"/>
+    <col customWidth="1" min="10" max="11" width="8.25"/>
+    <col customWidth="1" min="12" max="12" width="29.13"/>
+    <col customWidth="1" min="13" max="15" width="7.63"/>
+    <col customWidth="1" min="16" max="16" width="2.38"/>
+    <col customWidth="1" min="17" max="17" width="11.13"/>
+    <col customWidth="1" min="18" max="18" width="12.0"/>
+    <col customWidth="1" min="19" max="23" width="7.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="1">
@@ -595,496 +556,277 @@
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-      <c r="J1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="J1" s="5"/>
       <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="7"/>
+      <c r="L1" s="7"/>
     </row>
     <row r="2" ht="15.0" customHeight="1">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="4"/>
-      <c r="J2" s="11" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="9"/>
+      <c r="I2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="6"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
       <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="7"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="4"/>
-      <c r="J3" s="12" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="9"/>
+      <c r="I3" s="11" t="s">
         <v>5</v>
       </c>
+      <c r="J3" s="5"/>
       <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="13" t="s">
+      <c r="L3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="7"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="4"/>
-      <c r="J4" s="12" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="14"/>
+      <c r="I4" s="11" t="s">
         <v>8</v>
       </c>
+      <c r="J4" s="5"/>
       <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="13">
+      <c r="L4" s="12">
         <v>1.7</v>
       </c>
-      <c r="O4" s="7"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="4"/>
-      <c r="J5" s="12" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="16"/>
+      <c r="I5" s="11" t="s">
         <v>10</v>
       </c>
+      <c r="J5" s="5"/>
       <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="13">
+      <c r="L5" s="12">
         <v>6.0</v>
       </c>
-      <c r="O5" s="7"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="4"/>
-      <c r="J6" s="12"/>
+      <c r="A6" s="17"/>
+      <c r="D6" s="18"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="5"/>
       <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="7"/>
+      <c r="L6" s="12"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="4"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="6"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
       <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="4"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="16" t="s">
-        <v>12</v>
+      <c r="A9" s="20" t="s">
+        <v>11</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="18" t="s">
-        <v>13</v>
+      <c r="A10" s="20" t="s">
+        <v>12</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="16" t="s">
-        <v>14</v>
+      <c r="A11" s="20" t="s">
+        <v>13</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="16" t="s">
-        <v>15</v>
+      <c r="A12" s="20" t="s">
+        <v>14</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="20"/>
+      <c r="A13" s="22"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="20"/>
+      <c r="A14" s="22"/>
     </row>
     <row r="15" ht="24.0" customHeight="1">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="14"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="18"/>
     </row>
     <row r="16" ht="27.75" customHeight="1">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="C16" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="D16" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="E16" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="22" t="s">
+      <c r="F16" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="G16" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="22" t="s">
+      <c r="H16" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="22" t="s">
+      <c r="I16" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="22" t="s">
+      <c r="J16" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="J16" s="22" t="s">
+      <c r="K16" s="6"/>
+      <c r="L16" s="24" t="s">
         <v>25</v>
-      </c>
-      <c r="K16" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="L16" s="6"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="O16" s="22" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="17" ht="27.75" customHeight="1">
-      <c r="A17" s="24"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="22" t="s">
-        <v>29</v>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="24" t="s">
+        <v>26</v>
       </c>
-      <c r="L17" s="22" t="s">
-        <v>30</v>
+      <c r="K17" s="24" t="s">
+        <v>27</v>
       </c>
-      <c r="M17" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="N17" s="24"/>
-      <c r="O17" s="24"/>
+      <c r="L17" s="26"/>
     </row>
     <row r="18" ht="27.75" customHeight="1">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="25"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="26"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="32"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="28"/>
-      <c r="O19" s="28"/>
+    <row r="19" ht="15.75" customHeight="1"/>
+    <row r="20" ht="15.75" customHeight="1"/>
+    <row r="21" ht="15.75" customHeight="1"/>
+    <row r="22" ht="15.75" customHeight="1"/>
+    <row r="23" ht="15.75" customHeight="1"/>
+    <row r="24" ht="15.75" customHeight="1"/>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="T25" s="18"/>
+      <c r="U25" s="18"/>
+      <c r="V25" s="18"/>
+      <c r="W25" s="18"/>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="26"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="35"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="28"/>
-      <c r="O20" s="28"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="26"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="28"/>
-      <c r="O21" s="28"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="26"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="32"/>
-      <c r="M22" s="32"/>
-      <c r="N22" s="28"/>
-      <c r="O22" s="28"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="36"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="32"/>
-      <c r="M23" s="32"/>
-      <c r="N23" s="28"/>
-      <c r="O23" s="28"/>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="26"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="28"/>
-      <c r="O24" s="28"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="26"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="30"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="32"/>
-      <c r="M25" s="32"/>
-      <c r="N25" s="28"/>
-      <c r="O25" s="28"/>
-      <c r="P25" s="14"/>
-      <c r="Q25" s="14"/>
-      <c r="W25" s="14"/>
-      <c r="X25" s="14"/>
-      <c r="Y25" s="14"/>
-      <c r="Z25" s="14"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="26"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="30"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="31"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="32"/>
-      <c r="N26" s="28"/>
-      <c r="O26" s="28"/>
-    </row>
+    <row r="26" ht="15.75" customHeight="1"/>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="37"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="31"/>
-      <c r="L27" s="32"/>
-      <c r="M27" s="32"/>
-      <c r="N27" s="28"/>
-      <c r="O27" s="28"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-      <c r="W27" s="14"/>
-      <c r="X27" s="14"/>
-      <c r="Y27" s="14"/>
-      <c r="Z27" s="14"/>
+      <c r="T27" s="18"/>
+      <c r="U27" s="18"/>
+      <c r="V27" s="18"/>
+      <c r="W27" s="18"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="37"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="31"/>
-      <c r="L28" s="32"/>
-      <c r="M28" s="32"/>
-      <c r="N28" s="28"/>
-      <c r="O28" s="28"/>
-      <c r="P28" s="32"/>
-      <c r="Q28" s="32"/>
-      <c r="W28" s="32"/>
-      <c r="X28" s="32"/>
-      <c r="Y28" s="32"/>
-      <c r="Z28" s="32"/>
+      <c r="T28" s="28"/>
+      <c r="U28" s="28"/>
+      <c r="V28" s="28"/>
+      <c r="W28" s="28"/>
     </row>
     <row r="29" ht="15.75" customHeight="1"/>
     <row r="30" ht="15.75" customHeight="1"/>
@@ -2059,47 +1801,39 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="32">
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I7:L7"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="I1:K1"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="J2:O2"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="A13:O13"/>
-    <mergeCell ref="A14:O14"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="I2:L2"/>
     <mergeCell ref="A3:C3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="A13:L13"/>
+    <mergeCell ref="A14:L14"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="H16:H18"/>
+    <mergeCell ref="I16:I18"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:L18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="B16:B18"/>
     <mergeCell ref="C16:C18"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="N16:N18"/>
-    <mergeCell ref="O16:O18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="M17:M18"/>
     <mergeCell ref="D16:D18"/>
     <mergeCell ref="E16:E18"/>
     <mergeCell ref="F16:F18"/>
     <mergeCell ref="G16:G18"/>
-    <mergeCell ref="H16:H18"/>
-    <mergeCell ref="I16:I18"/>
-    <mergeCell ref="J16:J18"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.7480314960629921" footer="0.0" header="0.0" left="0.3937007874015748" right="0.31496062992125984" top="1.6535433070866143"/>

</xml_diff>